<commit_message>
creating unphotographed file, plus minor cleaning of other files
</commit_message>
<xml_diff>
--- a/data/master mismatches.xlsx
+++ b/data/master mismatches.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\GitHub\Australian-plant-photos\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D81E97-A41B-4478-B10D-C5D5729DD964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5069B260-B26A-47E7-A093-1697F1B2F8DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9945" yWindow="1905" windowWidth="28800" windowHeight="15435" xr2:uid="{E18B092A-E46D-49FE-B415-1528084BB7EE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{E18B092A-E46D-49FE-B415-1528084BB7EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4085" uniqueCount="1220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4110" uniqueCount="1225">
   <si>
     <t>iNaturalist_name</t>
   </si>
@@ -3695,6 +3695,21 @@
   </si>
   <si>
     <t>Amelichloa caudata</t>
+  </si>
+  <si>
+    <t>Cardiospermum halicacabum</t>
+  </si>
+  <si>
+    <t>Malvastrum coromandelianum</t>
+  </si>
+  <si>
+    <t>Malvastrum americanum</t>
+  </si>
+  <si>
+    <t>Spermacoce exilis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baeckea crassifolia </t>
   </si>
 </sst>
 </file>
@@ -4047,10 +4062,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD91070-41F0-4C24-BA04-4BAAA333C211}">
-  <dimension ref="A1:E817"/>
+  <dimension ref="A1:E822"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A688" workbookViewId="0">
-      <selection activeCell="A735" sqref="A735"/>
+    <sheetView tabSelected="1" topLeftCell="A797" workbookViewId="0">
+      <selection activeCell="E823" sqref="E823"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17951,6 +17966,91 @@
         <v>813</v>
       </c>
     </row>
+    <row r="818" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A818" t="s">
+        <v>1220</v>
+      </c>
+      <c r="B818" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C818" t="s">
+        <v>671</v>
+      </c>
+      <c r="D818" t="s">
+        <v>617</v>
+      </c>
+      <c r="E818" s="1" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="819" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A819" t="s">
+        <v>1221</v>
+      </c>
+      <c r="B819" t="s">
+        <v>1221</v>
+      </c>
+      <c r="C819" t="s">
+        <v>671</v>
+      </c>
+      <c r="D819" t="s">
+        <v>617</v>
+      </c>
+      <c r="E819" s="1" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="820" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A820" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B820" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C820" t="s">
+        <v>671</v>
+      </c>
+      <c r="D820" t="s">
+        <v>617</v>
+      </c>
+      <c r="E820" s="1" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="821" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A821" t="s">
+        <v>1223</v>
+      </c>
+      <c r="B821" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C821" t="s">
+        <v>671</v>
+      </c>
+      <c r="D821" t="s">
+        <v>617</v>
+      </c>
+      <c r="E821" s="1" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="822" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A822" t="s">
+        <v>72</v>
+      </c>
+      <c r="B822" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C822" t="s">
+        <v>655</v>
+      </c>
+      <c r="D822" t="s">
+        <v>617</v>
+      </c>
+      <c r="E822" s="1" t="s">
+        <v>813</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
assorted changes, fixed errors, new code etc relating to ala query
</commit_message>
<xml_diff>
--- a/data/master mismatches.xlsx
+++ b/data/master mismatches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\GitHub\Australian-plant-photos\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5069B260-B26A-47E7-A093-1697F1B2F8DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D29755-D16C-4095-B822-776B11DA6C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{E18B092A-E46D-49FE-B415-1528084BB7EE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4110" uniqueCount="1225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4185" uniqueCount="1257">
   <si>
     <t>iNaturalist_name</t>
   </si>
@@ -3710,16 +3710,125 @@
   </si>
   <si>
     <t xml:space="preserve">Baeckea crassifolia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Planchonella myrsinoides </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Planchonella pubescens </t>
+  </si>
+  <si>
+    <t>matched name should actually be Planchonella reticulata</t>
+  </si>
+  <si>
+    <t>Sphaeranthus indicus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heliotropium ovalifolium </t>
+  </si>
+  <si>
+    <t>Ocimum tenuiflorum</t>
+  </si>
+  <si>
+    <t>Boerhavia diffusa</t>
+  </si>
+  <si>
+    <t>Ipomoea aquatica</t>
+  </si>
+  <si>
+    <t>Carex echinata</t>
+  </si>
+  <si>
+    <t>Globba marantina</t>
+  </si>
+  <si>
+    <t>Paspalum vaginatum</t>
+  </si>
+  <si>
+    <t>Cucumis melo</t>
+  </si>
+  <si>
+    <t>Albizia procera</t>
+  </si>
+  <si>
+    <t>Eriosema chinense</t>
+  </si>
+  <si>
+    <t>Melochia corchorifolia</t>
+  </si>
+  <si>
+    <t>Alchemilla xanthochlora</t>
+  </si>
+  <si>
+    <t>Murraya paniculata</t>
+  </si>
+  <si>
+    <t>erroneously annotated as non-native on iNat</t>
+  </si>
+  <si>
+    <t>add to iM5</t>
+  </si>
+  <si>
+    <t>add to iM6</t>
+  </si>
+  <si>
+    <t>add to iM7</t>
+  </si>
+  <si>
+    <t>add to iM8</t>
+  </si>
+  <si>
+    <t>add to iM9</t>
+  </si>
+  <si>
+    <t>add to iM10</t>
+  </si>
+  <si>
+    <t>add to iM11</t>
+  </si>
+  <si>
+    <t>add to iM12</t>
+  </si>
+  <si>
+    <t>add to iM13</t>
+  </si>
+  <si>
+    <t>add to iM14</t>
+  </si>
+  <si>
+    <t>add to iM15</t>
+  </si>
+  <si>
+    <t>add to iM16</t>
+  </si>
+  <si>
+    <t>add to iM17</t>
+  </si>
+  <si>
+    <t>add to iM18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3745,9 +3854,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4062,10 +4172,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD91070-41F0-4C24-BA04-4BAAA333C211}">
-  <dimension ref="A1:E822"/>
+  <dimension ref="A1:E837"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A797" workbookViewId="0">
-      <selection activeCell="E823" sqref="E823"/>
+    <sheetView tabSelected="1" topLeftCell="A804" workbookViewId="0">
+      <selection activeCell="H830" sqref="H830"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18051,7 +18161,263 @@
         <v>813</v>
       </c>
     </row>
+    <row r="823" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A823" s="2" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B823" s="2" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C823" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D823" t="s">
+        <v>941</v>
+      </c>
+      <c r="E823" s="1" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="824" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A824" s="2" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B824" s="2" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C824" t="s">
+        <v>1242</v>
+      </c>
+      <c r="D824" t="s">
+        <v>1243</v>
+      </c>
+      <c r="E824" s="1" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="825" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A825" s="2" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B825" s="2" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C825" t="s">
+        <v>1242</v>
+      </c>
+      <c r="D825" t="s">
+        <v>1244</v>
+      </c>
+      <c r="E825" s="1" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="826" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A826" s="2" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B826" s="2" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C826" t="s">
+        <v>1242</v>
+      </c>
+      <c r="D826" t="s">
+        <v>1245</v>
+      </c>
+      <c r="E826" s="1" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="827" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A827" s="2" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B827" s="2" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C827" t="s">
+        <v>1242</v>
+      </c>
+      <c r="D827" t="s">
+        <v>1246</v>
+      </c>
+      <c r="E827" s="1" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="828" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A828" s="2" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B828" s="2" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C828" t="s">
+        <v>1242</v>
+      </c>
+      <c r="D828" t="s">
+        <v>1247</v>
+      </c>
+      <c r="E828" s="1" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="829" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A829" s="2" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B829" s="2" t="s">
+        <v>1233</v>
+      </c>
+      <c r="C829" t="s">
+        <v>1242</v>
+      </c>
+      <c r="D829" t="s">
+        <v>1248</v>
+      </c>
+      <c r="E829" s="1" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="830" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A830" s="2" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B830" s="2" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C830" t="s">
+        <v>1242</v>
+      </c>
+      <c r="D830" t="s">
+        <v>1249</v>
+      </c>
+      <c r="E830" s="1" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="831" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A831" s="2" t="s">
+        <v>1235</v>
+      </c>
+      <c r="B831" s="2" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C831" t="s">
+        <v>1242</v>
+      </c>
+      <c r="D831" t="s">
+        <v>1250</v>
+      </c>
+      <c r="E831" s="1" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="832" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A832" s="2" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B832" s="2" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C832" t="s">
+        <v>1242</v>
+      </c>
+      <c r="D832" t="s">
+        <v>1251</v>
+      </c>
+      <c r="E832" s="1" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="833" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A833" s="2" t="s">
+        <v>1237</v>
+      </c>
+      <c r="B833" s="2" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C833" t="s">
+        <v>1242</v>
+      </c>
+      <c r="D833" t="s">
+        <v>1252</v>
+      </c>
+      <c r="E833" s="1" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="834" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A834" s="2" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B834" s="2" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C834" t="s">
+        <v>1242</v>
+      </c>
+      <c r="D834" t="s">
+        <v>1253</v>
+      </c>
+      <c r="E834" s="1" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="835" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A835" s="2" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B835" s="2" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C835" t="s">
+        <v>1242</v>
+      </c>
+      <c r="D835" t="s">
+        <v>1254</v>
+      </c>
+      <c r="E835" s="1" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="836" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A836" s="2" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B836" s="2" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C836" t="s">
+        <v>1242</v>
+      </c>
+      <c r="D836" t="s">
+        <v>1255</v>
+      </c>
+      <c r="E836" s="1" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="837" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A837" s="2" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B837" s="2" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C837" t="s">
+        <v>1242</v>
+      </c>
+      <c r="D837" t="s">
+        <v>1256</v>
+      </c>
+      <c r="E837" s="1" t="s">
+        <v>813</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
assorted ala related changes
</commit_message>
<xml_diff>
--- a/data/master mismatches.xlsx
+++ b/data/master mismatches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\GitHub\Australian-plant-photos\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D29755-D16C-4095-B822-776B11DA6C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73AEB45C-1A73-4B3C-93B3-09E51D7AD2B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{E18B092A-E46D-49FE-B415-1528084BB7EE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4185" uniqueCount="1257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4190" uniqueCount="1247">
   <si>
     <t>iNaturalist_name</t>
   </si>
@@ -3769,43 +3769,13 @@
     <t>add to iM5</t>
   </si>
   <si>
-    <t>add to iM6</t>
-  </si>
-  <si>
-    <t>add to iM7</t>
-  </si>
-  <si>
-    <t>add to iM8</t>
-  </si>
-  <si>
-    <t>add to iM9</t>
-  </si>
-  <si>
-    <t>add to iM10</t>
-  </si>
-  <si>
-    <t>add to iM11</t>
-  </si>
-  <si>
-    <t>add to iM12</t>
-  </si>
-  <si>
-    <t>add to iM13</t>
-  </si>
-  <si>
-    <t>add to iM14</t>
-  </si>
-  <si>
-    <t>add to iM15</t>
-  </si>
-  <si>
-    <t>add to iM16</t>
-  </si>
-  <si>
-    <t>add to iM17</t>
-  </si>
-  <si>
-    <t>add to iM18</t>
+    <t>Callistemon pinifolius</t>
+  </si>
+  <si>
+    <t>didn't get matched</t>
+  </si>
+  <si>
+    <t>Melaleuca linearis acerosa</t>
   </si>
 </sst>
 </file>
@@ -4172,10 +4142,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD91070-41F0-4C24-BA04-4BAAA333C211}">
-  <dimension ref="A1:E837"/>
+  <dimension ref="A1:E838"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A804" workbookViewId="0">
-      <selection activeCell="H830" sqref="H830"/>
+      <selection activeCell="B847" sqref="B847"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18206,7 +18176,7 @@
         <v>1242</v>
       </c>
       <c r="D825" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="E825" s="1" t="s">
         <v>813</v>
@@ -18223,7 +18193,7 @@
         <v>1242</v>
       </c>
       <c r="D826" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="E826" s="1" t="s">
         <v>813</v>
@@ -18240,7 +18210,7 @@
         <v>1242</v>
       </c>
       <c r="D827" t="s">
-        <v>1246</v>
+        <v>1243</v>
       </c>
       <c r="E827" s="1" t="s">
         <v>813</v>
@@ -18257,7 +18227,7 @@
         <v>1242</v>
       </c>
       <c r="D828" t="s">
-        <v>1247</v>
+        <v>1243</v>
       </c>
       <c r="E828" s="1" t="s">
         <v>813</v>
@@ -18274,7 +18244,7 @@
         <v>1242</v>
       </c>
       <c r="D829" t="s">
-        <v>1248</v>
+        <v>1243</v>
       </c>
       <c r="E829" s="1" t="s">
         <v>813</v>
@@ -18291,7 +18261,7 @@
         <v>1242</v>
       </c>
       <c r="D830" t="s">
-        <v>1249</v>
+        <v>1243</v>
       </c>
       <c r="E830" s="1" t="s">
         <v>813</v>
@@ -18308,7 +18278,7 @@
         <v>1242</v>
       </c>
       <c r="D831" t="s">
-        <v>1250</v>
+        <v>1243</v>
       </c>
       <c r="E831" s="1" t="s">
         <v>813</v>
@@ -18325,7 +18295,7 @@
         <v>1242</v>
       </c>
       <c r="D832" t="s">
-        <v>1251</v>
+        <v>1243</v>
       </c>
       <c r="E832" s="1" t="s">
         <v>813</v>
@@ -18342,7 +18312,7 @@
         <v>1242</v>
       </c>
       <c r="D833" t="s">
-        <v>1252</v>
+        <v>1243</v>
       </c>
       <c r="E833" s="1" t="s">
         <v>813</v>
@@ -18359,7 +18329,7 @@
         <v>1242</v>
       </c>
       <c r="D834" t="s">
-        <v>1253</v>
+        <v>1243</v>
       </c>
       <c r="E834" s="1" t="s">
         <v>813</v>
@@ -18376,7 +18346,7 @@
         <v>1242</v>
       </c>
       <c r="D835" t="s">
-        <v>1254</v>
+        <v>1243</v>
       </c>
       <c r="E835" s="1" t="s">
         <v>813</v>
@@ -18393,7 +18363,7 @@
         <v>1242</v>
       </c>
       <c r="D836" t="s">
-        <v>1255</v>
+        <v>1243</v>
       </c>
       <c r="E836" s="1" t="s">
         <v>813</v>
@@ -18410,9 +18380,26 @@
         <v>1242</v>
       </c>
       <c r="D837" t="s">
-        <v>1256</v>
+        <v>1243</v>
       </c>
       <c r="E837" s="1" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="838" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A838" s="2" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B838" s="2" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C838" t="s">
+        <v>1245</v>
+      </c>
+      <c r="D838" t="s">
+        <v>1243</v>
+      </c>
+      <c r="E838" s="1" t="s">
         <v>813</v>
       </c>
     </row>

</xml_diff>